<commit_message>
Update in number label dimensions
</commit_message>
<xml_diff>
--- a/dist/game.xlsx
+++ b/dist/game.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25095" windowHeight="11910" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25095" windowHeight="11910" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="6">
   <si>
     <t>x</t>
   </si>
@@ -213,7 +214,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -225,6 +226,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -704,8 +709,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H7" sqref="A1:H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -895,4 +900,201 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="2">
+        <v>20</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="11">
+        <v>10</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="11">
+        <v>10</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="3">
+        <v>140</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="5">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="1">
+        <v>15</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" s="10">
+        <v>25</v>
+      </c>
+      <c r="H3" s="6">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="5">
+        <v>100</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="10">
+        <v>77</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="10">
+        <v>5</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="G5" s="10">
+        <v>115</v>
+      </c>
+      <c r="H5" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H6" s="14" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="7">
+        <v>9</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="8">
+        <v>4</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="8">
+        <v>3</v>
+      </c>
+      <c r="F7" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="G7" s="13">
+        <v>12</v>
+      </c>
+      <c r="H7" s="9">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>